<commit_message>
Added module breakdown table
</commit_message>
<xml_diff>
--- a/moduland_analysis/pathway_enrichment_data/module-analysis.xlsx
+++ b/moduland_analysis/pathway_enrichment_data/module-analysis.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Modules" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="568">
   <si>
     <t>module_priority</t>
   </si>
@@ -1708,6 +1708,18 @@
   </si>
   <si>
     <t>Deviation</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Pathway Description</t>
+  </si>
+  <si>
+    <t>Observed Gene Count</t>
+  </si>
+  <si>
+    <t>False Discovery Rate</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1763,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1776,8 +1788,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1796,11 +1814,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1832,6 +1879,23 @@
     </xf>
     <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1885,7 +1949,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$16</c:f>
+              <c:f>Modules!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1939,7 +2003,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$16</c:f>
+              <c:f>Modules!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2092,7 +2156,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$F$33</c:f>
+              <c:f>Modules!$F$19:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2146,7 +2210,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$33</c:f>
+              <c:f>Modules!$G$19:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2304,7 +2368,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$34:$F$40</c:f>
+              <c:f>Modules!$F$34:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2334,7 +2398,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$34:$G$40</c:f>
+              <c:f>Modules!$G$34:$G$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2458,7 +2522,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$41:$F$45</c:f>
+              <c:f>Modules!$F$41:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2482,7 +2546,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$41:$G$45</c:f>
+              <c:f>Modules!$G$41:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2600,7 +2664,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$46:$F$55</c:f>
+              <c:f>Modules!$F$46:$F$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2639,7 +2703,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$46:$G$55</c:f>
+              <c:f>Modules!$G$46:$G$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2777,7 +2841,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$56:$F$157</c:f>
+              <c:f>Modules!$F$56:$F$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="102"/>
@@ -3092,7 +3156,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$56:$G$157</c:f>
+              <c:f>Modules!$G$56:$G$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="102"/>
@@ -3501,7 +3565,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$158:$F$170</c:f>
+              <c:f>Modules!$F$158:$F$170</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3549,7 +3613,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$158:$G$170</c:f>
+              <c:f>Modules!$G$158:$G$170</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3691,7 +3755,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$171:$F$181</c:f>
+              <c:f>Modules!$F$171:$F$181</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3733,7 +3797,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$171:$G$181</c:f>
+              <c:f>Modules!$G$171:$G$181</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3874,7 +3938,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$182:$F$191</c:f>
+              <c:f>Modules!$F$182:$F$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3913,7 +3977,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$182:$G$191</c:f>
+              <c:f>Modules!$G$182:$G$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4256,16 +4320,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2981325</xdr:colOff>
-      <xdr:row>168</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>183</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4576,8 +4640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="K182" sqref="K182"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12481,12 +12545,785 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D218"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="84.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="18">
+        <v>3</v>
+      </c>
+      <c r="D2" s="19">
+        <v>5.2599999999999999E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="21">
+        <v>7</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1.0699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="21">
+        <v>6</v>
+      </c>
+      <c r="D4" s="22">
+        <v>3.5899999999999998E-12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="21">
+        <v>3</v>
+      </c>
+      <c r="D5" s="22">
+        <v>1.17E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="21">
+        <v>2</v>
+      </c>
+      <c r="D6" s="22">
+        <v>2.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="21">
+        <v>2</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1.2099999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="21">
+        <v>6</v>
+      </c>
+      <c r="D8" s="22">
+        <v>4.7800000000000004E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>488</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>500</v>
+      </c>
+      <c r="C9" s="21">
+        <v>4</v>
+      </c>
+      <c r="D9" s="22">
+        <v>9.9799999999999997E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>510</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>557</v>
+      </c>
+      <c r="C10" s="24">
+        <v>4</v>
+      </c>
+      <c r="D10" s="25">
+        <v>1.2100000000000001E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="6"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="6"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="6"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="6"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="6"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="6"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="6"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="6"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="6"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="6"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="6"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="6"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="6"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="6"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="6"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="6"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="6"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="6"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="6"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="6"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="6"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="6"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="6"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="6"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="6"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="6"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="6"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="6"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="6"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="6"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="6"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="6"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="6"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="6"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="6"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="6"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="6"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="6"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="6"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="6"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="6"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="6"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="6"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="6"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="6"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="6"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="6"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="6"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="6"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="6"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="6"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="6"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="6"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="6"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="6"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="6"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="6"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="6"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="6"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="6"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="6"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="6"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="6"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="6"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="6"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="6"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="6"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="6"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="6"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="6"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="6"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="6"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="6"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="6"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="6"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="6"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="6"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="6"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="6"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="6"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="6"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="6"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="6"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="6"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="6"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="6"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="6"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="6"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="6"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="6"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="6"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="6"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="6"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="6"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="6"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="6"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="6"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="6"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="6"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="6"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="6"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="6"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="6"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="6"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="6"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="6"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="6"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="6"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="6"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="6"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="6"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="6"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="6"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="6"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="6"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="6"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="6"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="6"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="6"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="6"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="6"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="6"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="6"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="6"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="6"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="6"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="6"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="6"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="6"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="6"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="6"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="6"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="6"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="6"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="6"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>